<commit_message>
Discussion on 30th April
</commit_message>
<xml_diff>
--- a/inputs/E_CigO_fordiscussion.xlsx
+++ b/inputs/E_CigO_fordiscussion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Documents\GitHub\addiction-ontology\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A82C0D70-3480-4631-8BC5-6C6CDCFC8E81}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC98EC09-D1DE-475F-9426-158BAE9F7F51}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CFD89471-969D-DA4E-B695-10E28209D64F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="83">
   <si>
     <t>ID</t>
   </si>
@@ -235,13 +235,52 @@
   </si>
   <si>
     <t>A government agency that muddies the waters on definition of tobacco products</t>
+  </si>
+  <si>
+    <t>A tobacco smoker who participates in tobacco smoking very day.</t>
+  </si>
+  <si>
+    <t>Past 30-day tobacco smoker</t>
+  </si>
+  <si>
+    <t>This refers to a current time frame for participation. This should be specified unless it is obviousl from context.</t>
+  </si>
+  <si>
+    <t>An ever-tobacco smoker who has participated in tobacco smoking within the past 30 days.</t>
+  </si>
+  <si>
+    <t>Ever-tobacco smoker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This includes any participation, including one puff on a single cigarette. It is in references to a current time frame that needs to be specfified unless it is bvious from the context. </t>
+  </si>
+  <si>
+    <t>Tobacco smoker identity</t>
+  </si>
+  <si>
+    <t>A mental representation that a person has about themselves.</t>
+  </si>
+  <si>
+    <t>Core identity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An identity </t>
+  </si>
+  <si>
+    <t>Self identity</t>
+  </si>
+  <si>
+    <t>The term 'self' sounds tautologous but is required to reflect the fact that this is not identity in terms of who you are but how you represent yourself to yourself.</t>
+  </si>
+  <si>
+    <t>An identity that in which a person represents themselves as a tobacco smoker.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -281,6 +320,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -302,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -332,6 +377,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -648,10 +696,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2F1A1D6-CE09-5741-871E-C0900D993FE1}">
-  <dimension ref="A1:T24"/>
+  <dimension ref="A1:T28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -791,7 +842,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="10" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" s="10" customFormat="1" ht="108.5" x14ac:dyDescent="0.35">
       <c r="B5" s="10" t="s">
         <v>42</v>
       </c>
@@ -807,226 +858,282 @@
       <c r="F5" s="10" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="C6" s="9" t="s">
+      <c r="K5" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" s="10" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="C6" s="10" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="C7" s="9" t="s">
+      <c r="D6" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" s="10" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="C7" s="10" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" s="10" customFormat="1" ht="108.5" x14ac:dyDescent="0.35">
-      <c r="B8" s="10" t="s">
+      <c r="D7" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" s="10" customFormat="1" ht="170.5" x14ac:dyDescent="0.35">
+      <c r="C8" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" s="11" customFormat="1" ht="124" x14ac:dyDescent="0.35">
+      <c r="C9" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" s="11" customFormat="1" ht="62" x14ac:dyDescent="0.35">
+      <c r="C11" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" s="10" customFormat="1" ht="108.5" x14ac:dyDescent="0.35">
+      <c r="B12" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C12" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D12" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E12" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:20" s="10" customFormat="1" ht="124" x14ac:dyDescent="0.35">
-      <c r="C9" s="10" t="s">
+    <row r="13" spans="1:20" s="10" customFormat="1" ht="124" x14ac:dyDescent="0.35">
+      <c r="C13" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D13" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E13" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="B10" s="9" t="s">
+    <row r="14" spans="1:20" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="B14" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C14" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D14" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E14" s="9" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="C11" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" s="10" customFormat="1" ht="108.5" x14ac:dyDescent="0.35">
-      <c r="C12" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" ht="62" x14ac:dyDescent="0.35">
-      <c r="B13" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" ht="31" x14ac:dyDescent="0.35">
-      <c r="B14" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="C15" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" s="10" customFormat="1" ht="108.5" x14ac:dyDescent="0.35">
+      <c r="C16" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="62" x14ac:dyDescent="0.35">
+      <c r="B17" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="31" x14ac:dyDescent="0.35">
+      <c r="B18" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="C19" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="B16" s="9" t="s">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B20" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C20" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B17" s="9" t="s">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B21" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C21" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B18" s="9" t="s">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B22" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C22" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:19" s="7" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5" t="s">
+    <row r="23" spans="1:19" s="7" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C23" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D23" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E23" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F23" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G23" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5" t="s">
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="K19" s="6"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5">
+      <c r="K23" s="6"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5">
         <v>1</v>
       </c>
-      <c r="P19" s="5" t="s">
+      <c r="P23" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="Q19" s="5" t="s">
+      <c r="Q23" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="R19" s="5"/>
-    </row>
-    <row r="20" spans="1:19" s="7" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="B20" s="7" t="s">
+      <c r="R23" s="5"/>
+    </row>
+    <row r="24" spans="1:19" s="7" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="B24" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C24" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D24" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E24" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5" t="s">
+      <c r="F24" s="5"/>
+      <c r="G24" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
-      <c r="P20" s="5" t="s">
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="Q20" s="5" t="s">
+      <c r="Q24" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="R20" s="5"/>
-      <c r="S20" s="6"/>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="C21" s="9" t="s">
+      <c r="R24" s="5"/>
+      <c r="S24" s="6"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="C25" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="31" x14ac:dyDescent="0.35">
-      <c r="B22" s="9" t="s">
+    <row r="26" spans="1:19" ht="31" x14ac:dyDescent="0.35">
+      <c r="B26" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C26" s="9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B23" s="9" t="s">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B27" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C27" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B24" s="9" t="s">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B28" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C28" s="9" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding discussed definitions to correct files
</commit_message>
<xml_diff>
--- a/inputs/E_CigO_fordiscussion.xlsx
+++ b/inputs/E_CigO_fordiscussion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Documents\GitHub\addiction-ontology\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sharoncox/Documents/GitHub/addiction-ontology/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626C4751-E36D-483D-884B-8C859B5DA5E2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6D57DD-71C6-8241-A256-BD961A918C92}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CFD89471-969D-DA4E-B695-10E28209D64F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{CFD89471-969D-DA4E-B695-10E28209D64F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="128">
   <si>
     <t>ID</t>
   </si>
@@ -406,6 +406,9 @@
   </si>
   <si>
     <t>Identity</t>
+  </si>
+  <si>
+    <t>*</t>
   </si>
 </sst>
 </file>
@@ -818,19 +821,19 @@
   <dimension ref="A1:U33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomRight" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="10.6640625" style="6"/>
     <col min="3" max="3" width="27.33203125" style="6" customWidth="1"/>
     <col min="4" max="4" width="23.83203125" style="6" customWidth="1"/>
     <col min="5" max="5" width="21" style="6" customWidth="1"/>
-    <col min="6" max="6" width="17.9140625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" style="6" customWidth="1"/>
     <col min="7" max="7" width="16.83203125" style="6" customWidth="1"/>
     <col min="8" max="8" width="17" style="6" customWidth="1"/>
     <col min="9" max="9" width="18.33203125" style="6" customWidth="1"/>
@@ -847,7 +850,7 @@
     <col min="21" max="16384" width="10.6640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -912,7 +915,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
@@ -935,7 +938,10 @@
       <c r="T2" s="1"/>
       <c r="U2" s="2"/>
     </row>
-    <row r="3" spans="1:21" s="7" customFormat="1" ht="62" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" s="7" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="B3" s="7" t="s">
         <v>42</v>
       </c>
@@ -952,7 +958,10 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="7" customFormat="1" ht="62" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" s="7" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="B4" s="7" t="s">
         <v>42</v>
       </c>
@@ -969,7 +978,10 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:21" s="7" customFormat="1" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" s="7" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="B5" s="7" t="s">
         <v>38</v>
       </c>
@@ -989,7 +1001,10 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="7" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" s="7" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="C6" s="7" t="s">
         <v>56</v>
       </c>
@@ -1000,7 +1015,10 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:21" s="7" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" s="7" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="C7" s="7" t="s">
         <v>57</v>
       </c>
@@ -1011,7 +1029,10 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:21" s="7" customFormat="1" ht="170.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" s="7" customFormat="1" ht="187" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="C8" s="7" t="s">
         <v>65</v>
       </c>
@@ -1025,7 +1046,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="7" customFormat="1" ht="201.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" s="7" customFormat="1" ht="221" x14ac:dyDescent="0.2">
       <c r="C9" s="7" t="s">
         <v>73</v>
       </c>
@@ -1042,7 +1063,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="7" customFormat="1" ht="62" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" s="7" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="C10" s="7" t="s">
         <v>72</v>
       </c>
@@ -1053,7 +1074,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="7" customFormat="1" ht="124" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" s="7" customFormat="1" ht="153" x14ac:dyDescent="0.2">
       <c r="C11" s="7" t="s">
         <v>70</v>
       </c>
@@ -1064,7 +1085,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:21" s="7" customFormat="1" ht="62" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" s="7" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="C12" s="7" t="s">
         <v>82</v>
       </c>
@@ -1075,7 +1096,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="7" customFormat="1" ht="62" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" s="7" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="C13" s="7" t="s">
         <v>84</v>
       </c>
@@ -1083,7 +1104,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:21" s="7" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" s="7" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="C14" s="7" t="s">
         <v>122</v>
       </c>
@@ -1097,7 +1118,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:21" s="7" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" s="7" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="C15" s="7" t="s">
         <v>78</v>
       </c>
@@ -1105,7 +1126,10 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:21" s="7" customFormat="1" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" s="7" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="B16" s="7" t="s">
         <v>37</v>
       </c>
@@ -1119,7 +1143,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:20" s="7" customFormat="1" ht="124" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" s="7" customFormat="1" ht="136" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="C17" s="7" t="s">
         <v>54</v>
       </c>
@@ -1130,7 +1157,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:20" s="7" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:20" s="7" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="B18" s="7" t="s">
         <v>38</v>
       </c>
@@ -1144,7 +1174,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:20" s="7" customFormat="1" ht="62" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:20" s="7" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="C19" s="7" t="s">
         <v>59</v>
       </c>
@@ -1158,7 +1191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:20" s="7" customFormat="1" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:20" s="7" customFormat="1" ht="119" x14ac:dyDescent="0.2">
       <c r="C20" s="7" t="s">
         <v>19</v>
       </c>
@@ -1172,7 +1205,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:20" s="7" customFormat="1" ht="62" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:20" s="7" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="B21" s="7" t="s">
         <v>34</v>
       </c>
@@ -1189,7 +1222,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:20" s="7" customFormat="1" ht="310" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:20" s="7" customFormat="1" ht="340" x14ac:dyDescent="0.2">
       <c r="B22" s="7" t="s">
         <v>91</v>
       </c>
@@ -1206,7 +1239,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
         <v>34</v>
       </c>
@@ -1220,7 +1253,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="1:20" s="7" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:20" s="7" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="C24" s="7" t="s">
         <v>20</v>
       </c>
@@ -1231,7 +1264,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:20" s="7" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:20" s="7" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="C25" s="7" t="s">
         <v>98</v>
       </c>
@@ -1242,7 +1275,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:20" s="7" customFormat="1" ht="139.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:20" s="7" customFormat="1" ht="170" x14ac:dyDescent="0.2">
       <c r="B26" s="7" t="s">
         <v>37</v>
       </c>
@@ -1262,7 +1295,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:20" s="7" customFormat="1" ht="139.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:20" s="7" customFormat="1" ht="153" x14ac:dyDescent="0.2">
       <c r="B27" s="7" t="s">
         <v>37</v>
       </c>
@@ -1282,7 +1315,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="28" spans="1:20" s="7" customFormat="1" ht="139.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:20" s="7" customFormat="1" ht="153" x14ac:dyDescent="0.2">
       <c r="B28" s="7" t="s">
         <v>37</v>
       </c>
@@ -1299,8 +1332,10 @@
         <v>112</v>
       </c>
     </row>
-    <row r="29" spans="1:20" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A29" s="2"/>
+    <row r="29" spans="1:20" s="1" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="B29" s="2" t="s">
         <v>25</v>
       </c>
@@ -1340,7 +1375,7 @@
       </c>
       <c r="S29" s="2"/>
     </row>
-    <row r="30" spans="1:20" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:20" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>34</v>
       </c>
@@ -1375,7 +1410,10 @@
       <c r="S30" s="2"/>
       <c r="T30" s="3"/>
     </row>
-    <row r="31" spans="1:20" s="7" customFormat="1" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:20" s="7" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+      <c r="A31" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="C31" s="7" t="s">
         <v>23</v>
       </c>
@@ -1389,7 +1427,10 @@
         <v>115</v>
       </c>
     </row>
-    <row r="32" spans="1:20" s="7" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:20" s="7" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A32" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="B32" s="7" t="s">
         <v>38</v>
       </c>
@@ -1403,7 +1444,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="33" spans="2:12" s="7" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:12" s="7" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="B33" s="7" t="s">
         <v>37</v>
       </c>

</xml_diff>